<commit_message>
small update to variable names
</commit_message>
<xml_diff>
--- a/project1/data_structures.xlsx
+++ b/project1/data_structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\TXSTATE UNI\Fall 2022\Artificial Intelligence\Projects\artificial_intelligence\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C9672D-A55D-41E2-8992-55B70F135353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EA8908-62B7-41B2-96E6-1CBA217454B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0FDAD4B7-6A52-43B5-89AE-0D674C76519E}"/>
+    <workbookView xWindow="-11415" yWindow="-11880" windowWidth="16725" windowHeight="7170" xr2:uid="{0FDAD4B7-6A52-43B5-89AE-0D674C76519E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="214">
   <si>
     <t>Variable Name</t>
   </si>
@@ -452,9 +452,6 @@
     <t>1, 5, 16, 39</t>
   </si>
   <si>
-    <t>THEN PART = FUEL</t>
-  </si>
-  <si>
     <t>IF PROBLEM = YES AND ENGINE_ROTATES = YES AND FUEL = YES</t>
   </si>
   <si>
@@ -675,6 +672,12 @@
   </si>
   <si>
     <t>Clause Variable List</t>
+  </si>
+  <si>
+    <t>THEN PART = FUEL_LEVEL</t>
+  </si>
+  <si>
+    <t>THEN PART = FUEL_CONDITION</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61881F8C-F8C7-4282-985C-88E013F6406E}">
   <dimension ref="A1:C1933"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1939" sqref="B1939"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,7 +1426,7 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C36">
         <v>69</v>
@@ -1784,7 +1787,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>138</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -1792,15 +1795,15 @@
         <v>150</v>
       </c>
       <c r="B79" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" t="s">
         <v>139</v>
-      </c>
-      <c r="C79" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -1808,15 +1811,15 @@
         <v>160</v>
       </c>
       <c r="B81" t="s">
+        <v>141</v>
+      </c>
+      <c r="C81" t="s">
         <v>142</v>
-      </c>
-      <c r="C81" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -1824,15 +1827,15 @@
         <v>170</v>
       </c>
       <c r="B83" t="s">
+        <v>144</v>
+      </c>
+      <c r="C83" t="s">
         <v>145</v>
-      </c>
-      <c r="C83" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -1840,15 +1843,15 @@
         <v>180</v>
       </c>
       <c r="B85" t="s">
+        <v>147</v>
+      </c>
+      <c r="C85" t="s">
         <v>148</v>
-      </c>
-      <c r="C85" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>138</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -1856,15 +1859,15 @@
         <v>190</v>
       </c>
       <c r="B87" t="s">
+        <v>149</v>
+      </c>
+      <c r="C87" t="s">
         <v>150</v>
-      </c>
-      <c r="C87" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -1872,15 +1875,15 @@
         <v>200</v>
       </c>
       <c r="B89" t="s">
+        <v>152</v>
+      </c>
+      <c r="C89" t="s">
         <v>153</v>
-      </c>
-      <c r="C89" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -1888,15 +1891,15 @@
         <v>210</v>
       </c>
       <c r="B91" t="s">
+        <v>155</v>
+      </c>
+      <c r="C91" t="s">
         <v>156</v>
-      </c>
-      <c r="C91" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -1904,10 +1907,10 @@
         <v>220</v>
       </c>
       <c r="B93" t="s">
+        <v>158</v>
+      </c>
+      <c r="C93" t="s">
         <v>159</v>
-      </c>
-      <c r="C93" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -1920,15 +1923,15 @@
         <v>230</v>
       </c>
       <c r="B95" t="s">
+        <v>160</v>
+      </c>
+      <c r="C95" t="s">
         <v>161</v>
-      </c>
-      <c r="C95" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -1936,15 +1939,15 @@
         <v>240</v>
       </c>
       <c r="B97" t="s">
+        <v>163</v>
+      </c>
+      <c r="C97" t="s">
         <v>164</v>
-      </c>
-      <c r="C97" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -1952,15 +1955,15 @@
         <v>250</v>
       </c>
       <c r="B99" t="s">
+        <v>166</v>
+      </c>
+      <c r="C99" t="s">
         <v>167</v>
-      </c>
-      <c r="C99" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -1968,15 +1971,15 @@
         <v>260</v>
       </c>
       <c r="B101" t="s">
+        <v>169</v>
+      </c>
+      <c r="C101" t="s">
         <v>170</v>
-      </c>
-      <c r="C101" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -1984,15 +1987,15 @@
         <v>270</v>
       </c>
       <c r="B103" t="s">
+        <v>172</v>
+      </c>
+      <c r="C103" t="s">
         <v>173</v>
-      </c>
-      <c r="C103" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -2000,15 +2003,15 @@
         <v>280</v>
       </c>
       <c r="B105" t="s">
+        <v>175</v>
+      </c>
+      <c r="C105" t="s">
         <v>176</v>
-      </c>
-      <c r="C105" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -2016,10 +2019,10 @@
         <v>290</v>
       </c>
       <c r="B107" t="s">
+        <v>178</v>
+      </c>
+      <c r="C107" t="s">
         <v>179</v>
-      </c>
-      <c r="C107" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -2032,15 +2035,15 @@
         <v>300</v>
       </c>
       <c r="B109" t="s">
+        <v>181</v>
+      </c>
+      <c r="C109" t="s">
         <v>182</v>
-      </c>
-      <c r="C109" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -2048,15 +2051,15 @@
         <v>310</v>
       </c>
       <c r="B111" t="s">
+        <v>184</v>
+      </c>
+      <c r="C111" t="s">
         <v>185</v>
-      </c>
-      <c r="C111" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -2064,15 +2067,15 @@
         <v>320</v>
       </c>
       <c r="B113" t="s">
+        <v>187</v>
+      </c>
+      <c r="C113" t="s">
         <v>188</v>
-      </c>
-      <c r="C113" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -2080,15 +2083,15 @@
         <v>330</v>
       </c>
       <c r="B115" t="s">
+        <v>190</v>
+      </c>
+      <c r="C115" t="s">
         <v>191</v>
-      </c>
-      <c r="C115" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -2096,15 +2099,15 @@
         <v>340</v>
       </c>
       <c r="B117" t="s">
+        <v>193</v>
+      </c>
+      <c r="C117" t="s">
         <v>194</v>
-      </c>
-      <c r="C117" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -2112,15 +2115,15 @@
         <v>350</v>
       </c>
       <c r="B119" t="s">
+        <v>195</v>
+      </c>
+      <c r="C119" t="s">
         <v>196</v>
-      </c>
-      <c r="C119" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -2128,15 +2131,15 @@
         <v>360</v>
       </c>
       <c r="B121" t="s">
+        <v>199</v>
+      </c>
+      <c r="C121" t="s">
         <v>200</v>
-      </c>
-      <c r="C121" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -2144,15 +2147,15 @@
         <v>370</v>
       </c>
       <c r="B123" t="s">
+        <v>202</v>
+      </c>
+      <c r="C123" t="s">
         <v>203</v>
-      </c>
-      <c r="C123" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -2160,15 +2163,15 @@
         <v>380</v>
       </c>
       <c r="B125" t="s">
+        <v>204</v>
+      </c>
+      <c r="C125" t="s">
         <v>205</v>
-      </c>
-      <c r="C125" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -2176,20 +2179,20 @@
         <v>390</v>
       </c>
       <c r="B127" t="s">
+        <v>206</v>
+      </c>
+      <c r="C127" t="s">
         <v>207</v>
-      </c>
-      <c r="C127" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -2506,7 +2509,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -2863,7 +2866,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>